<commit_message>
small mod to Overview page
</commit_message>
<xml_diff>
--- a/prototype/alr_ig/output/StructureDefinition-ext-changeReason.xlsx
+++ b/prototype/alr_ig/output/StructureDefinition-ext-changeReason.xlsx
@@ -6,16 +6,116 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Elements" r:id="rId3" sheetId="1"/>
+    <sheet name="Metadata" r:id="rId3" sheetId="1"/>
+    <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$11</definedName>
-  </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="110">
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://alr.cms.gov/ig/StructureDefinition/ext-changeReason</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ChangeReason</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>ALR Change Reason</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Experimental</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2021-12-10T11:55:44-07:00</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ALR Change Reason Description</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Copyright</t>
+  </si>
+  <si>
+    <t>FHIR Version</t>
+  </si>
+  <si>
+    <t>4.0.1</t>
+  </si>
+  <si>
+    <t>Kind</t>
+  </si>
+  <si>
+    <t>complex-type</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>Base Definition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/Extension</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Derivation</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>element:Element</t>
+  </si>
   <si>
     <t>Path</t>
   </si>
@@ -125,9 +225,6 @@
     <t>Mapping: RIM Mapping</t>
   </si>
   <si>
-    <t>Extension</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -135,12 +232,6 @@
   </si>
   <si>
     <t>*</t>
-  </si>
-  <si>
-    <t>ALR Change Reason</t>
-  </si>
-  <si>
-    <t>ALR Change Reason Description</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
@@ -258,9 +349,6 @@
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
-  </si>
-  <si>
-    <t>http://alr.cms.gov/ig/StructureDefinition/ext-changeReason</t>
   </si>
   <si>
     <t>base64Binary
@@ -393,29 +481,175 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color indexed="22"/>
-        <i val="true"/>
-      </font>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="true"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="15.703125" customWidth="true"/>
+    <col min="2" max="2" width="80.703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true">
+    <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -462,1141 +696,1123 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="Z1" t="s" s="1">
+        <v>59</v>
+      </c>
+      <c r="AA1" t="s" s="1">
+        <v>60</v>
+      </c>
+      <c r="AB1" t="s" s="1">
+        <v>61</v>
+      </c>
+      <c r="AC1" t="s" s="1">
+        <v>62</v>
+      </c>
+      <c r="AD1" t="s" s="1">
+        <v>63</v>
+      </c>
+      <c r="AE1" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="AF1" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="AG1" t="s" s="1">
+        <v>66</v>
+      </c>
+      <c r="AH1" t="s" s="1">
+        <v>67</v>
+      </c>
+      <c r="AI1" t="s" s="1">
+        <v>68</v>
+      </c>
+      <c r="AJ1" t="s" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
         <v>25</v>
-      </c>
-      <c r="AA1" t="s" s="1">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s" s="1">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s" s="1">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s" s="1">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s" s="1">
-        <v>33</v>
-      </c>
-      <c r="AI1" t="s" s="1">
-        <v>34</v>
-      </c>
-      <c r="AJ1" t="s" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" hidden="true">
-      <c r="A2" t="s" s="2">
-        <v>36</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="R2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="S2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="T2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="U2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="X2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Y2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Z2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AA2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AC2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AD2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="AG2" t="s" s="2">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" hidden="true">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s" s="2">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="R3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="X3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Y3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Z3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AA3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AD3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" hidden="true">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s" s="2">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="R4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" hidden="true">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s" s="2">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="R5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AB5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AC5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AD5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" hidden="true">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s" s="2">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="R6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="V6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AC6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" hidden="true">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s" s="2">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="R7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="S7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="T7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="U7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="V7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="W7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="X7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Y7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Z7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AA7" t="s" s="2">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="AB7" t="s" s="2">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="AC7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AD7" t="s" s="2">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="AG7" t="s" s="2">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" hidden="true">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s" s="2">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" t="s" s="2">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="R8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="S8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="T8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="U8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="V8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="W8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="X8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Y8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Z8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AA8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AB8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AC8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AD8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="AH8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" hidden="true">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s" s="2">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="R9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="S9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="T9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="U9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="V9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="W9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="X9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Y9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Z9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AE9" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="AF9" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AG9" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="AF9" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG9" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="AH9" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" hidden="true">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s" s="2">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" t="s" s="2">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="R10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="S10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="T10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="U10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="V10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="W10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="X10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Y10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Z10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AA10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AC10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="AG10" t="s" s="2">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" hidden="true">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s" s="2">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="R11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="S11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="T11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="U11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="V11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="Z11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AA11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AB11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AC11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AD11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AE11" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="AF11" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AG11" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="AF11" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AG11" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="AH11" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>71</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ11">
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="26">
-      <filters blank="true"/>
-    </filterColumn>
-  </autoFilter>
-  <conditionalFormatting sqref="A2:AI10">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$G2&lt;&gt;"Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$Q2&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>